<commit_message>
Creación Scripts y descargables con ERROR 24/08/2025
</commit_message>
<xml_diff>
--- a/02.descargable/XLSX/01.XLSX correctos/reseñas.xlsx
+++ b/02.descargable/XLSX/01.XLSX correctos/reseñas.xlsx
@@ -477,12 +477,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C-000873</t>
+          <t>C-001531</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CL-02303</t>
+          <t>CL-05513</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -490,11 +490,11 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Muy buen producto, llegó rápido.</t>
+          <t>Me encantó, lo recomiendo.</t>
         </is>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45890</v>
+        <v>45889</v>
       </c>
     </row>
     <row r="3">
@@ -505,24 +505,24 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>C-002514</t>
+          <t>C-000291</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CL-02665</t>
+          <t>CL-02529</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Volveré a comprar sin duda.</t>
+          <t>No era lo que esperaba.</t>
         </is>
       </c>
       <c r="F3" s="2" t="n">
-        <v>45890</v>
+        <v>45859</v>
       </c>
     </row>
     <row r="4">
@@ -533,24 +533,24 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>C-003576</t>
+          <t>C-001221</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CL-05157</t>
+          <t>CL-01649</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Volveré a comprar sin duda.</t>
+          <t>La talla no era correcta.</t>
         </is>
       </c>
       <c r="F4" s="2" t="n">
-        <v>45856</v>
+        <v>45851</v>
       </c>
     </row>
     <row r="5">
@@ -561,24 +561,24 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>C-000343</t>
+          <t>C-001760</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CL-03797</t>
+          <t>CL-05951</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Tuve problemas con la entrega.</t>
+          <t>Me encantó, lo recomiendo.</t>
         </is>
       </c>
       <c r="F5" s="2" t="n">
-        <v>45838</v>
+        <v>45882</v>
       </c>
     </row>
     <row r="6">
@@ -589,16 +589,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>C-002195</t>
+          <t>C-000752</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CL-07760</t>
+          <t>CL-04106</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -606,7 +606,7 @@
         </is>
       </c>
       <c r="F6" s="2" t="n">
-        <v>45875</v>
+        <v>45866</v>
       </c>
     </row>
     <row r="7">
@@ -617,24 +617,24 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>C-000153</t>
+          <t>C-002352</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CL-06407</t>
+          <t>CL-02900</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>No era lo que esperaba.</t>
+          <t>Muy buen producto, llegó rápido.</t>
         </is>
       </c>
       <c r="F7" s="2" t="n">
-        <v>45865</v>
+        <v>45866</v>
       </c>
     </row>
     <row r="8">
@@ -645,12 +645,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>C-000901</t>
+          <t>C-002756</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CL-06440</t>
+          <t>CL-05673</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -658,11 +658,11 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>El embalaje estaba dañado.</t>
+          <t>Volveré a comprar sin duda.</t>
         </is>
       </c>
       <c r="F8" s="2" t="n">
-        <v>45865</v>
+        <v>45851</v>
       </c>
     </row>
     <row r="9">
@@ -673,12 +673,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>C-003923</t>
+          <t>C-004561</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CL-01646</t>
+          <t>CL-07335</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -686,11 +686,11 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Todo perfecto, gracias.</t>
+          <t>Volveré a comprar sin duda.</t>
         </is>
       </c>
       <c r="F9" s="2" t="n">
-        <v>45892</v>
+        <v>45882</v>
       </c>
     </row>
     <row r="10">
@@ -701,24 +701,24 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>C-000928</t>
+          <t>C-004025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CL-00847</t>
+          <t>CL-01907</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>El embalaje estaba dañado.</t>
+          <t>Precio justo y buena calidad.</t>
         </is>
       </c>
       <c r="F10" s="2" t="n">
-        <v>45881</v>
+        <v>45867</v>
       </c>
     </row>
     <row r="11">
@@ -729,12 +729,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>C-000487</t>
+          <t>C-001563</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CL-05052</t>
+          <t>CL-05770</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -742,11 +742,11 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>No era lo que esperaba.</t>
+          <t>Muy buen producto, llegó rápido.</t>
         </is>
       </c>
       <c r="F11" s="2" t="n">
-        <v>45829</v>
+        <v>45869</v>
       </c>
     </row>
     <row r="12">
@@ -757,24 +757,24 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>C-001193</t>
+          <t>C-003004</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CL-03652</t>
+          <t>CL-08389</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Precio justo y buena calidad.</t>
+          <t>Excelente atención al cliente.</t>
         </is>
       </c>
       <c r="F12" s="2" t="n">
-        <v>45881</v>
+        <v>45844</v>
       </c>
     </row>
     <row r="13">
@@ -785,24 +785,24 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>C-001477</t>
+          <t>C-004855</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CL-05042</t>
+          <t>CL-05023</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>La talla no era correcta.</t>
+          <t>Todo perfecto, gracias.</t>
         </is>
       </c>
       <c r="F13" s="2" t="n">
-        <v>45871</v>
+        <v>45890</v>
       </c>
     </row>
     <row r="14">
@@ -813,24 +813,24 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>C-003447</t>
+          <t>C-001289</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>CL-03400</t>
+          <t>CL-03861</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>El embalaje estaba dañado.</t>
+          <t>Volveré a comprar sin duda.</t>
         </is>
       </c>
       <c r="F14" s="2" t="n">
-        <v>45878</v>
+        <v>45832</v>
       </c>
     </row>
     <row r="15">
@@ -841,24 +841,24 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>C-001188</t>
+          <t>C-002931</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>CL-00255</t>
+          <t>CL-04253</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>No era lo que esperaba.</t>
+          <t>La talla no era correcta.</t>
         </is>
       </c>
       <c r="F15" s="2" t="n">
-        <v>45877</v>
+        <v>45872</v>
       </c>
     </row>
     <row r="16">
@@ -869,24 +869,24 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>C-001152</t>
+          <t>C-001078</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>CL-05265</t>
+          <t>CL-09696</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Me encantó, lo recomiendo.</t>
+          <t>Excelente atención al cliente.</t>
         </is>
       </c>
       <c r="F16" s="2" t="n">
-        <v>45872</v>
+        <v>45828</v>
       </c>
     </row>
     <row r="17">
@@ -897,24 +897,24 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>C-003983</t>
+          <t>C-000366</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>CL-07674</t>
+          <t>CL-06730</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Me encantó, lo recomiendo.</t>
+          <t>No era lo que esperaba.</t>
         </is>
       </c>
       <c r="F17" s="2" t="n">
-        <v>45871</v>
+        <v>45888</v>
       </c>
     </row>
     <row r="18">
@@ -925,24 +925,24 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>C-002992</t>
+          <t>C-000337</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>CL-07076</t>
+          <t>CL-08441</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Todo perfecto, gracias.</t>
+          <t>Tuve problemas con la entrega.</t>
         </is>
       </c>
       <c r="F18" s="2" t="n">
-        <v>45837</v>
+        <v>45846</v>
       </c>
     </row>
     <row r="19">
@@ -953,24 +953,24 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>C-004547</t>
+          <t>C-002730</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>CL-03237</t>
+          <t>CL-05065</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>No era lo que esperaba.</t>
+          <t>Volveré a comprar sin duda.</t>
         </is>
       </c>
       <c r="F19" s="2" t="n">
-        <v>45882</v>
+        <v>45853</v>
       </c>
     </row>
     <row r="20">
@@ -981,12 +981,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>C-002780</t>
+          <t>C-000611</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>CL-03826</t>
+          <t>CL-08139</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -994,11 +994,11 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>El embalaje estaba dañado.</t>
+          <t>Excelente atención al cliente.</t>
         </is>
       </c>
       <c r="F20" s="2" t="n">
-        <v>45878</v>
+        <v>45876</v>
       </c>
     </row>
     <row r="21">
@@ -1009,24 +1009,24 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>C-000621</t>
+          <t>C-002700</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CL-05785</t>
+          <t>CL-09913</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Me encantó, lo recomiendo.</t>
+          <t>Muy buen producto, llegó rápido.</t>
         </is>
       </c>
       <c r="F21" s="2" t="n">
-        <v>45867</v>
+        <v>45869</v>
       </c>
     </row>
     <row r="22">
@@ -1037,24 +1037,24 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>C-001766</t>
+          <t>C-002490</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>CL-09952</t>
+          <t>CL-06599</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>El embalaje estaba dañado.</t>
+          <t>Todo perfecto, gracias.</t>
         </is>
       </c>
       <c r="F22" s="2" t="n">
-        <v>45831</v>
+        <v>45879</v>
       </c>
     </row>
     <row r="23">
@@ -1065,24 +1065,24 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>C-004564</t>
+          <t>C-004573</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>CL-07722</t>
+          <t>CL-01518</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Tuve problemas con la entrega.</t>
+          <t>Muy buen producto, llegó rápido.</t>
         </is>
       </c>
       <c r="F23" s="2" t="n">
-        <v>45884</v>
+        <v>45879</v>
       </c>
     </row>
     <row r="24">
@@ -1093,24 +1093,24 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>C-002279</t>
+          <t>C-003615</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>CL-02572</t>
+          <t>CL-02749</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Precio justo y buena calidad.</t>
+          <t>Muy buen producto, llegó rápido.</t>
         </is>
       </c>
       <c r="F24" s="2" t="n">
-        <v>45823</v>
+        <v>45855</v>
       </c>
     </row>
     <row r="25">
@@ -1121,12 +1121,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>C-000766</t>
+          <t>C-004319</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>CL-07140</t>
+          <t>CL-05066</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1134,11 +1134,11 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>No era lo que esperaba.</t>
+          <t>Precio justo y buena calidad.</t>
         </is>
       </c>
       <c r="F25" s="2" t="n">
-        <v>45861</v>
+        <v>45876</v>
       </c>
     </row>
     <row r="26">
@@ -1149,12 +1149,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>C-002642</t>
+          <t>C-002674</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CL-07789</t>
+          <t>CL-05641</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1162,11 +1162,11 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Me encantó, lo recomiendo.</t>
+          <t>No era lo que esperaba.</t>
         </is>
       </c>
       <c r="F26" s="2" t="n">
-        <v>45856</v>
+        <v>45892</v>
       </c>
     </row>
     <row r="27">
@@ -1177,24 +1177,24 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>C-000717</t>
+          <t>C-001849</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CL-02341</t>
+          <t>CL-02455</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Volveré a comprar sin duda.</t>
+          <t>La talla no era correcta.</t>
         </is>
       </c>
       <c r="F27" s="2" t="n">
-        <v>45880</v>
+        <v>45842</v>
       </c>
     </row>
     <row r="28">
@@ -1205,12 +1205,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>C-004700</t>
+          <t>C-003253</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CL-06868</t>
+          <t>CL-09604</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1218,11 +1218,11 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Excelente atención al cliente.</t>
+          <t>No era lo que esperaba.</t>
         </is>
       </c>
       <c r="F28" s="2" t="n">
-        <v>45873</v>
+        <v>45879</v>
       </c>
     </row>
     <row r="29">
@@ -1233,24 +1233,24 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>C-003845</t>
+          <t>C-002550</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CL-00789</t>
+          <t>CL-08286</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>La talla no era correcta.</t>
+          <t>Precio justo y buena calidad.</t>
         </is>
       </c>
       <c r="F29" s="2" t="n">
-        <v>45886</v>
+        <v>45881</v>
       </c>
     </row>
     <row r="30">
@@ -1261,24 +1261,24 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>C-003246</t>
+          <t>C-000179</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>CL-07183</t>
+          <t>CL-01545</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>La talla no era correcta.</t>
+          <t>El embalaje estaba dañado.</t>
         </is>
       </c>
       <c r="F30" s="2" t="n">
-        <v>45890</v>
+        <v>45881</v>
       </c>
     </row>
     <row r="31">
@@ -1289,24 +1289,24 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>C-002147</t>
+          <t>C-004899</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>CL-05616</t>
+          <t>CL-00291</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Tuve problemas con la entrega.</t>
+          <t>Excelente atención al cliente.</t>
         </is>
       </c>
       <c r="F31" s="2" t="n">
-        <v>45889</v>
+        <v>45858</v>
       </c>
     </row>
     <row r="32">
@@ -1317,12 +1317,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>C-000724</t>
+          <t>C-001552</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>CL-01008</t>
+          <t>CL-02886</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1330,11 +1330,11 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Tuve problemas con la entrega.</t>
+          <t>El embalaje estaba dañado.</t>
         </is>
       </c>
       <c r="F32" s="2" t="n">
-        <v>45878</v>
+        <v>45836</v>
       </c>
     </row>
     <row r="33">
@@ -1345,12 +1345,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>C-003113</t>
+          <t>C-003230</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>CL-08477</t>
+          <t>CL-09322</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1358,11 +1358,11 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Excelente atención al cliente.</t>
+          <t>El embalaje estaba dañado.</t>
         </is>
       </c>
       <c r="F33" s="2" t="n">
-        <v>45883</v>
+        <v>45888</v>
       </c>
     </row>
     <row r="34">
@@ -1373,12 +1373,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>C-000630</t>
+          <t>C-000864</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>CL-06074</t>
+          <t>CL-01765</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1386,7 +1386,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Tuve problemas con la entrega.</t>
+          <t>La talla no era correcta.</t>
         </is>
       </c>
       <c r="F34" s="2" t="n">
@@ -1401,12 +1401,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>C-002372</t>
+          <t>C-000751</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>CL-06589</t>
+          <t>CL-09774</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1414,11 +1414,11 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Me encantó, lo recomiendo.</t>
+          <t>El embalaje estaba dañado.</t>
         </is>
       </c>
       <c r="F35" s="2" t="n">
-        <v>45888</v>
+        <v>45864</v>
       </c>
     </row>
     <row r="36">
@@ -1429,24 +1429,24 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>C-002102</t>
+          <t>C-002046</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>CL-07421</t>
+          <t>CL-05289</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Me encantó, lo recomiendo.</t>
+          <t>Muy buen producto, llegó rápido.</t>
         </is>
       </c>
       <c r="F36" s="2" t="n">
-        <v>45877</v>
+        <v>45892</v>
       </c>
     </row>
     <row r="37">
@@ -1457,24 +1457,24 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>C-001799</t>
+          <t>C-000939</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>CL-06436</t>
+          <t>CL-00715</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Excelente atención al cliente.</t>
+          <t>Volveré a comprar sin duda.</t>
         </is>
       </c>
       <c r="F37" s="2" t="n">
-        <v>45845</v>
+        <v>45892</v>
       </c>
     </row>
     <row r="38">
@@ -1485,24 +1485,24 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>C-002964</t>
+          <t>C-001166</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>CL-09290</t>
+          <t>CL-05699</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Precio justo y buena calidad.</t>
+          <t>Muy buen producto, llegó rápido.</t>
         </is>
       </c>
       <c r="F38" s="2" t="n">
-        <v>45887</v>
+        <v>45877</v>
       </c>
     </row>
     <row r="39">
@@ -1513,24 +1513,24 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>C-000025</t>
+          <t>C-003085</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>CL-00911</t>
+          <t>CL-08434</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>La talla no era correcta.</t>
+          <t>No era lo que esperaba.</t>
         </is>
       </c>
       <c r="F39" s="2" t="n">
-        <v>45875</v>
+        <v>45886</v>
       </c>
     </row>
     <row r="40">
@@ -1541,24 +1541,24 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>C-002737</t>
+          <t>C-003497</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>CL-06070</t>
+          <t>CL-06058</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Tuve problemas con la entrega.</t>
+          <t>Todo perfecto, gracias.</t>
         </is>
       </c>
       <c r="F40" s="2" t="n">
-        <v>45881</v>
+        <v>45856</v>
       </c>
     </row>
     <row r="41">
@@ -1569,24 +1569,24 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>C-001084</t>
+          <t>C-001787</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>CL-03523</t>
+          <t>CL-02816</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>La talla no era correcta.</t>
+          <t>Me encantó, lo recomiendo.</t>
         </is>
       </c>
       <c r="F41" s="2" t="n">
-        <v>45871</v>
+        <v>45835</v>
       </c>
     </row>
     <row r="42">
@@ -1597,12 +1597,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>C-002238</t>
+          <t>C-002542</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>CL-00663</t>
+          <t>CL-03835</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1610,11 +1610,11 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>El embalaje estaba dañado.</t>
+          <t>No era lo que esperaba.</t>
         </is>
       </c>
       <c r="F42" s="2" t="n">
-        <v>45864</v>
+        <v>45884</v>
       </c>
     </row>
     <row r="43">
@@ -1625,16 +1625,16 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>C-001300</t>
+          <t>C-004801</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>CL-04787</t>
+          <t>CL-05193</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1642,7 +1642,7 @@
         </is>
       </c>
       <c r="F43" s="2" t="n">
-        <v>45859</v>
+        <v>45869</v>
       </c>
     </row>
     <row r="44">
@@ -1653,24 +1653,24 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>C-003589</t>
+          <t>C-001011</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>CL-04033</t>
+          <t>CL-01722</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Todo perfecto, gracias.</t>
+          <t>Muy buen producto, llegó rápido.</t>
         </is>
       </c>
       <c r="F44" s="2" t="n">
-        <v>45839</v>
+        <v>45892</v>
       </c>
     </row>
     <row r="45">
@@ -1681,20 +1681,20 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>C-003925</t>
+          <t>C-001108</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>CL-07557</t>
+          <t>CL-03245</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Tuve problemas con la entrega.</t>
+          <t>La talla no era correcta.</t>
         </is>
       </c>
       <c r="F45" s="2" t="n">
@@ -1709,12 +1709,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>C-001342</t>
+          <t>C-003469</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>CL-08084</t>
+          <t>CL-08773</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1722,11 +1722,11 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Volveré a comprar sin duda.</t>
+          <t>Me encantó, lo recomiendo.</t>
         </is>
       </c>
       <c r="F46" s="2" t="n">
-        <v>45859</v>
+        <v>45839</v>
       </c>
     </row>
     <row r="47">
@@ -1737,24 +1737,24 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>C-000623</t>
+          <t>C-002405</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>CL-05982</t>
+          <t>CL-06087</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Tuve problemas con la entrega.</t>
+          <t>Muy buen producto, llegó rápido.</t>
         </is>
       </c>
       <c r="F47" s="2" t="n">
-        <v>45887</v>
+        <v>45880</v>
       </c>
     </row>
     <row r="48">
@@ -1765,24 +1765,24 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>C-003069</t>
+          <t>C-004122</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>CL-09980</t>
+          <t>CL-08221</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Precio justo y buena calidad.</t>
+          <t>Me encantó, lo recomiendo.</t>
         </is>
       </c>
       <c r="F48" s="2" t="n">
-        <v>45832</v>
+        <v>45846</v>
       </c>
     </row>
     <row r="49">
@@ -1793,12 +1793,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>C-000883</t>
+          <t>C-001488</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>CL-04679</t>
+          <t>CL-03641</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1806,11 +1806,11 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>No era lo que esperaba.</t>
+          <t>Excelente atención al cliente.</t>
         </is>
       </c>
       <c r="F49" s="2" t="n">
-        <v>45890</v>
+        <v>45858</v>
       </c>
     </row>
     <row r="50">
@@ -1821,12 +1821,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>C-000589</t>
+          <t>C-000527</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>CL-02992</t>
+          <t>CL-03028</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1834,11 +1834,11 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Me encantó, lo recomiendo.</t>
+          <t>Volveré a comprar sin duda.</t>
         </is>
       </c>
       <c r="F50" s="2" t="n">
-        <v>45892</v>
+        <v>45891</v>
       </c>
     </row>
     <row r="51">
@@ -1849,24 +1849,24 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>C-003486</t>
+          <t>C-003594</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>CL-07475</t>
+          <t>CL-07854</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Me encantó, lo recomiendo.</t>
+          <t>El embalaje estaba dañado.</t>
         </is>
       </c>
       <c r="F51" s="2" t="n">
-        <v>45845</v>
+        <v>45889</v>
       </c>
     </row>
     <row r="52">
@@ -1877,12 +1877,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>C-001942</t>
+          <t>C-001654</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>CL-00493</t>
+          <t>CL-01729</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1890,11 +1890,11 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Me encantó, lo recomiendo.</t>
+          <t>Volveré a comprar sin duda.</t>
         </is>
       </c>
       <c r="F52" s="2" t="n">
-        <v>45863</v>
+        <v>45887</v>
       </c>
     </row>
     <row r="53">
@@ -1905,12 +1905,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>C-003514</t>
+          <t>C-003580</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>CL-06173</t>
+          <t>CL-09301</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1918,11 +1918,11 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Tuve problemas con la entrega.</t>
+          <t>No era lo que esperaba.</t>
         </is>
       </c>
       <c r="F53" s="2" t="n">
-        <v>45890</v>
+        <v>45871</v>
       </c>
     </row>
     <row r="54">
@@ -1933,12 +1933,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>C-002300</t>
+          <t>C-001028</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>CL-00510</t>
+          <t>CL-07341</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1946,11 +1946,11 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Muy buen producto, llegó rápido.</t>
+          <t>No era lo que esperaba.</t>
         </is>
       </c>
       <c r="F54" s="2" t="n">
-        <v>45883</v>
+        <v>45887</v>
       </c>
     </row>
     <row r="55">
@@ -1961,24 +1961,24 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>C-002520</t>
+          <t>C-002679</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>CL-01648</t>
+          <t>CL-07068</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>El embalaje estaba dañado.</t>
+          <t>Precio justo y buena calidad.</t>
         </is>
       </c>
       <c r="F55" s="2" t="n">
-        <v>45884</v>
+        <v>45811</v>
       </c>
     </row>
     <row r="56">
@@ -1989,24 +1989,24 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>C-002349</t>
+          <t>C-002900</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>CL-08693</t>
+          <t>CL-00839</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Todo perfecto, gracias.</t>
+          <t>Muy buen producto, llegó rápido.</t>
         </is>
       </c>
       <c r="F56" s="2" t="n">
-        <v>45833</v>
+        <v>45885</v>
       </c>
     </row>
     <row r="57">
@@ -2017,12 +2017,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>C-000652</t>
+          <t>C-003202</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>CL-01782</t>
+          <t>CL-07955</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2030,11 +2030,11 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Precio justo y buena calidad.</t>
+          <t>La talla no era correcta.</t>
         </is>
       </c>
       <c r="F57" s="2" t="n">
-        <v>45849</v>
+        <v>45888</v>
       </c>
     </row>
     <row r="58">
@@ -2045,24 +2045,24 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>C-001548</t>
+          <t>C-003940</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>CL-07815</t>
+          <t>CL-01377</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Precio justo y buena calidad.</t>
+          <t>Me encantó, lo recomiendo.</t>
         </is>
       </c>
       <c r="F58" s="2" t="n">
-        <v>45864</v>
+        <v>45861</v>
       </c>
     </row>
     <row r="59">
@@ -2073,24 +2073,24 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>C-004676</t>
+          <t>C-001244</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>CL-04869</t>
+          <t>CL-04645</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Tuve problemas con la entrega.</t>
+          <t>Todo perfecto, gracias.</t>
         </is>
       </c>
       <c r="F59" s="2" t="n">
-        <v>45890</v>
+        <v>45835</v>
       </c>
     </row>
     <row r="60">
@@ -2101,24 +2101,24 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>C-004183</t>
+          <t>C-003363</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>CL-07678</t>
+          <t>CL-06142</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Todo perfecto, gracias.</t>
+          <t>Precio justo y buena calidad.</t>
         </is>
       </c>
       <c r="F60" s="2" t="n">
-        <v>45876</v>
+        <v>45880</v>
       </c>
     </row>
     <row r="61">
@@ -2129,12 +2129,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>C-004401</t>
+          <t>C-001451</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>CL-01204</t>
+          <t>CL-03402</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -2146,7 +2146,7 @@
         </is>
       </c>
       <c r="F61" s="2" t="n">
-        <v>45860</v>
+        <v>45843</v>
       </c>
     </row>
     <row r="62">
@@ -2157,16 +2157,16 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>C-002409</t>
+          <t>C-000705</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>CL-00437</t>
+          <t>CL-06792</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2174,7 +2174,7 @@
         </is>
       </c>
       <c r="F62" s="2" t="n">
-        <v>45870</v>
+        <v>45892</v>
       </c>
     </row>
     <row r="63">
@@ -2185,24 +2185,24 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>C-000352</t>
+          <t>C-000469</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>CL-07041</t>
+          <t>CL-09450</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>No era lo que esperaba.</t>
+          <t>Muy buen producto, llegó rápido.</t>
         </is>
       </c>
       <c r="F63" s="2" t="n">
-        <v>45847</v>
+        <v>45863</v>
       </c>
     </row>
     <row r="64">
@@ -2213,24 +2213,24 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>C-002044</t>
+          <t>C-003535</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>CL-05324</t>
+          <t>CL-04452</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Me encantó, lo recomiendo.</t>
+          <t>Precio justo y buena calidad.</t>
         </is>
       </c>
       <c r="F64" s="2" t="n">
-        <v>45882</v>
+        <v>45874</v>
       </c>
     </row>
     <row r="65">
@@ -2241,24 +2241,24 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>C-002954</t>
+          <t>C-000830</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>CL-08865</t>
+          <t>CL-08829</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Muy buen producto, llegó rápido.</t>
+          <t>Precio justo y buena calidad.</t>
         </is>
       </c>
       <c r="F65" s="2" t="n">
-        <v>45890</v>
+        <v>45884</v>
       </c>
     </row>
     <row r="66">
@@ -2269,24 +2269,24 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>C-002915</t>
+          <t>C-003508</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>CL-07605</t>
+          <t>CL-01494</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Muy buen producto, llegó rápido.</t>
+          <t>Precio justo y buena calidad.</t>
         </is>
       </c>
       <c r="F66" s="2" t="n">
-        <v>45884</v>
+        <v>45873</v>
       </c>
     </row>
     <row r="67">
@@ -2297,24 +2297,24 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>C-004506</t>
+          <t>C-001361</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>CL-05627</t>
+          <t>CL-02515</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>No era lo que esperaba.</t>
+          <t>La talla no era correcta.</t>
         </is>
       </c>
       <c r="F67" s="2" t="n">
-        <v>45892</v>
+        <v>45871</v>
       </c>
     </row>
     <row r="68">
@@ -2325,16 +2325,16 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>C-002531</t>
+          <t>C-001519</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>CL-03478</t>
+          <t>CL-06912</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2342,7 +2342,7 @@
         </is>
       </c>
       <c r="F68" s="2" t="n">
-        <v>45855</v>
+        <v>45878</v>
       </c>
     </row>
     <row r="69">
@@ -2353,12 +2353,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>C-003417</t>
+          <t>C-002007</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>CL-05816</t>
+          <t>CL-07749</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -2366,11 +2366,11 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Todo perfecto, gracias.</t>
+          <t>La talla no era correcta.</t>
         </is>
       </c>
       <c r="F69" s="2" t="n">
-        <v>45876</v>
+        <v>45873</v>
       </c>
     </row>
     <row r="70">
@@ -2381,24 +2381,24 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>C-002411</t>
+          <t>C-002844</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>CL-05368</t>
+          <t>CL-09295</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Muy buen producto, llegó rápido.</t>
+          <t>Precio justo y buena calidad.</t>
         </is>
       </c>
       <c r="F70" s="2" t="n">
-        <v>45849</v>
+        <v>45870</v>
       </c>
     </row>
     <row r="71">
@@ -2409,24 +2409,24 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>C-002477</t>
+          <t>C-004945</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>CL-07426</t>
+          <t>CL-02578</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Todo perfecto, gracias.</t>
+          <t>No era lo que esperaba.</t>
         </is>
       </c>
       <c r="F71" s="2" t="n">
-        <v>45864</v>
+        <v>45847</v>
       </c>
     </row>
     <row r="72">
@@ -2437,12 +2437,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>C-002756</t>
+          <t>C-002204</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>CL-09698</t>
+          <t>CL-07621</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -2450,11 +2450,11 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>La talla no era correcta.</t>
+          <t>Muy buen producto, llegó rápido.</t>
         </is>
       </c>
       <c r="F72" s="2" t="n">
-        <v>45886</v>
+        <v>45861</v>
       </c>
     </row>
     <row r="73">
@@ -2465,24 +2465,24 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>C-004162</t>
+          <t>C-003923</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>CL-03784</t>
+          <t>CL-00965</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Precio justo y buena calidad.</t>
+          <t>La talla no era correcta.</t>
         </is>
       </c>
       <c r="F73" s="2" t="n">
-        <v>45879</v>
+        <v>45891</v>
       </c>
     </row>
     <row r="74">
@@ -2493,12 +2493,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>C-004729</t>
+          <t>C-004652</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>CL-09769</t>
+          <t>CL-04033</t>
         </is>
       </c>
       <c r="D74" t="n">
@@ -2506,11 +2506,11 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Tuve problemas con la entrega.</t>
+          <t>La talla no era correcta.</t>
         </is>
       </c>
       <c r="F74" s="2" t="n">
-        <v>45824</v>
+        <v>45890</v>
       </c>
     </row>
     <row r="75">
@@ -2521,12 +2521,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>C-001038</t>
+          <t>C-004922</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>CL-01834</t>
+          <t>CL-09867</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2534,11 +2534,11 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Volveré a comprar sin duda.</t>
+          <t>Excelente atención al cliente.</t>
         </is>
       </c>
       <c r="F75" s="2" t="n">
-        <v>45872</v>
+        <v>45876</v>
       </c>
     </row>
     <row r="76">
@@ -2549,12 +2549,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>C-004929</t>
+          <t>C-004498</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>CL-09040</t>
+          <t>CL-01368</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2562,11 +2562,11 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Todo perfecto, gracias.</t>
+          <t>Excelente atención al cliente.</t>
         </is>
       </c>
       <c r="F76" s="2" t="n">
-        <v>45873</v>
+        <v>45874</v>
       </c>
     </row>
     <row r="77">
@@ -2577,24 +2577,24 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>C-004820</t>
+          <t>C-001883</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>CL-08433</t>
+          <t>CL-06660</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>No era lo que esperaba.</t>
+          <t>Tuve problemas con la entrega.</t>
         </is>
       </c>
       <c r="F77" s="2" t="n">
-        <v>45891</v>
+        <v>45872</v>
       </c>
     </row>
     <row r="78">
@@ -2605,24 +2605,24 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>C-001758</t>
+          <t>C-002354</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>CL-07104</t>
+          <t>CL-09388</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>La talla no era correcta.</t>
+          <t>Volveré a comprar sin duda.</t>
         </is>
       </c>
       <c r="F78" s="2" t="n">
-        <v>45890</v>
+        <v>45866</v>
       </c>
     </row>
     <row r="79">
@@ -2633,12 +2633,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>C-003348</t>
+          <t>C-000648</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>CL-00759</t>
+          <t>CL-06984</t>
         </is>
       </c>
       <c r="D79" t="n">
@@ -2646,11 +2646,11 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Excelente atención al cliente.</t>
+          <t>Me encantó, lo recomiendo.</t>
         </is>
       </c>
       <c r="F79" s="2" t="n">
-        <v>45874</v>
+        <v>45878</v>
       </c>
     </row>
     <row r="80">
@@ -2661,24 +2661,24 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>C-004612</t>
+          <t>C-001645</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>CL-03182</t>
+          <t>CL-01734</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Me encantó, lo recomiendo.</t>
+          <t>Excelente atención al cliente.</t>
         </is>
       </c>
       <c r="F80" s="2" t="n">
-        <v>45884</v>
+        <v>45868</v>
       </c>
     </row>
     <row r="81">
@@ -2689,24 +2689,24 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>C-001920</t>
+          <t>C-003412</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>CL-06832</t>
+          <t>CL-00746</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Tuve problemas con la entrega.</t>
+          <t>Me encantó, lo recomiendo.</t>
         </is>
       </c>
       <c r="F81" s="2" t="n">
-        <v>45873</v>
+        <v>45875</v>
       </c>
     </row>
     <row r="82">
@@ -2717,24 +2717,24 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>C-002051</t>
+          <t>C-000196</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>CL-00407</t>
+          <t>CL-04467</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Volveré a comprar sin duda.</t>
+          <t>Me encantó, lo recomiendo.</t>
         </is>
       </c>
       <c r="F82" s="2" t="n">
-        <v>45872</v>
+        <v>45869</v>
       </c>
     </row>
     <row r="83">
@@ -2745,12 +2745,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>C-004159</t>
+          <t>C-002432</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>CL-03583</t>
+          <t>CL-02989</t>
         </is>
       </c>
       <c r="D83" t="n">
@@ -2762,7 +2762,7 @@
         </is>
       </c>
       <c r="F83" s="2" t="n">
-        <v>45892</v>
+        <v>45888</v>
       </c>
     </row>
     <row r="84">
@@ -2773,24 +2773,24 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>C-000929</t>
+          <t>C-004035</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>CL-00462</t>
+          <t>CL-02340</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Todo perfecto, gracias.</t>
+          <t>No era lo que esperaba.</t>
         </is>
       </c>
       <c r="F84" s="2" t="n">
-        <v>45858</v>
+        <v>45853</v>
       </c>
     </row>
     <row r="85">
@@ -2801,24 +2801,24 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>C-001706</t>
+          <t>C-000707</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>CL-02371</t>
+          <t>CL-00080</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Precio justo y buena calidad.</t>
+          <t>Volveré a comprar sin duda.</t>
         </is>
       </c>
       <c r="F85" s="2" t="n">
-        <v>45884</v>
+        <v>45867</v>
       </c>
     </row>
     <row r="86">
@@ -2829,24 +2829,24 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>C-002493</t>
+          <t>C-001136</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>CL-00157</t>
+          <t>CL-09780</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Precio justo y buena calidad.</t>
+          <t>Todo perfecto, gracias.</t>
         </is>
       </c>
       <c r="F86" s="2" t="n">
-        <v>45824</v>
+        <v>45848</v>
       </c>
     </row>
     <row r="87">
@@ -2857,12 +2857,12 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>C-004127</t>
+          <t>C-000191</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>CL-02136</t>
+          <t>CL-06860</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2870,11 +2870,11 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Todo perfecto, gracias.</t>
+          <t>Precio justo y buena calidad.</t>
         </is>
       </c>
       <c r="F87" s="2" t="n">
-        <v>45864</v>
+        <v>45879</v>
       </c>
     </row>
     <row r="88">
@@ -2885,12 +2885,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>C-003694</t>
+          <t>C-004958</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>CL-06833</t>
+          <t>CL-05231</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2898,11 +2898,11 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Me encantó, lo recomiendo.</t>
+          <t>Precio justo y buena calidad.</t>
         </is>
       </c>
       <c r="F88" s="2" t="n">
-        <v>45875</v>
+        <v>45866</v>
       </c>
     </row>
     <row r="89">
@@ -2913,24 +2913,24 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>C-002460</t>
+          <t>C-004291</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>CL-04481</t>
+          <t>CL-04178</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Me encantó, lo recomiendo.</t>
+          <t>Volveré a comprar sin duda.</t>
         </is>
       </c>
       <c r="F89" s="2" t="n">
-        <v>45870</v>
+        <v>45873</v>
       </c>
     </row>
     <row r="90">
@@ -2941,24 +2941,24 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>C-001177</t>
+          <t>C-000685</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>CL-04740</t>
+          <t>CL-00136</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Tuve problemas con la entrega.</t>
+          <t>Precio justo y buena calidad.</t>
         </is>
       </c>
       <c r="F90" s="2" t="n">
-        <v>45812</v>
+        <v>45886</v>
       </c>
     </row>
     <row r="91">
@@ -2969,24 +2969,24 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>C-002577</t>
+          <t>C-002932</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>CL-01505</t>
+          <t>CL-08041</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Precio justo y buena calidad.</t>
+          <t>No era lo que esperaba.</t>
         </is>
       </c>
       <c r="F91" s="2" t="n">
-        <v>45831</v>
+        <v>45858</v>
       </c>
     </row>
     <row r="92">
@@ -2997,24 +2997,24 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>C-000511</t>
+          <t>C-002434</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>CL-02514</t>
+          <t>CL-05886</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Precio justo y buena calidad.</t>
+          <t>La talla no era correcta.</t>
         </is>
       </c>
       <c r="F92" s="2" t="n">
-        <v>45888</v>
+        <v>45883</v>
       </c>
     </row>
     <row r="93">
@@ -3025,24 +3025,24 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>C-002661</t>
+          <t>C-003415</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>CL-02610</t>
+          <t>CL-05645</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Me encantó, lo recomiendo.</t>
+          <t>No era lo que esperaba.</t>
         </is>
       </c>
       <c r="F93" s="2" t="n">
-        <v>45882</v>
+        <v>45887</v>
       </c>
     </row>
     <row r="94">
@@ -3053,24 +3053,24 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>C-003943</t>
+          <t>C-004651</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>CL-05557</t>
+          <t>CL-06335</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>La talla no era correcta.</t>
+          <t>Volveré a comprar sin duda.</t>
         </is>
       </c>
       <c r="F94" s="2" t="n">
-        <v>45891</v>
+        <v>45847</v>
       </c>
     </row>
     <row r="95">
@@ -3081,12 +3081,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>C-000259</t>
+          <t>C-000766</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>CL-06557</t>
+          <t>CL-09380</t>
         </is>
       </c>
       <c r="D95" t="n">
@@ -3094,11 +3094,11 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>La talla no era correcta.</t>
+          <t>Precio justo y buena calidad.</t>
         </is>
       </c>
       <c r="F95" s="2" t="n">
-        <v>45872</v>
+        <v>45892</v>
       </c>
     </row>
     <row r="96">
@@ -3109,24 +3109,24 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>C-004163</t>
+          <t>C-003296</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>CL-03034</t>
+          <t>CL-01165</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Excelente atención al cliente.</t>
+          <t>Volveré a comprar sin duda.</t>
         </is>
       </c>
       <c r="F96" s="2" t="n">
-        <v>45889</v>
+        <v>45854</v>
       </c>
     </row>
     <row r="97">
@@ -3137,16 +3137,16 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>C-002426</t>
+          <t>C-003297</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>CL-02707</t>
+          <t>CL-00221</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -3154,7 +3154,7 @@
         </is>
       </c>
       <c r="F97" s="2" t="n">
-        <v>45892</v>
+        <v>45875</v>
       </c>
     </row>
     <row r="98">
@@ -3165,12 +3165,12 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>C-004255</t>
+          <t>C-002023</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>CL-06031</t>
+          <t>CL-09962</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -3178,11 +3178,11 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Tuve problemas con la entrega.</t>
+          <t>No era lo que esperaba.</t>
         </is>
       </c>
       <c r="F98" s="2" t="n">
-        <v>45892</v>
+        <v>45885</v>
       </c>
     </row>
     <row r="99">
@@ -3193,24 +3193,24 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>C-004268</t>
+          <t>C-001431</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>CL-05355</t>
+          <t>CL-06350</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>El embalaje estaba dañado.</t>
+          <t>Muy buen producto, llegó rápido.</t>
         </is>
       </c>
       <c r="F99" s="2" t="n">
-        <v>45890</v>
+        <v>45871</v>
       </c>
     </row>
     <row r="100">
@@ -3221,12 +3221,12 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>C-001174</t>
+          <t>C-003811</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>CL-09068</t>
+          <t>CL-00101</t>
         </is>
       </c>
       <c r="D100" t="n">
@@ -3234,11 +3234,11 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Excelente atención al cliente.</t>
+          <t>Me encantó, lo recomiendo.</t>
         </is>
       </c>
       <c r="F100" s="2" t="n">
-        <v>45891</v>
+        <v>45865</v>
       </c>
     </row>
     <row r="101">
@@ -3249,24 +3249,24 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>C-003105</t>
+          <t>C-003287</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>CL-04163</t>
+          <t>CL-00179</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Muy buen producto, llegó rápido.</t>
+          <t>No era lo que esperaba.</t>
         </is>
       </c>
       <c r="F101" s="2" t="n">
-        <v>45870</v>
+        <v>45839</v>
       </c>
     </row>
   </sheetData>

</xml_diff>